<commit_message>
- adicionados alguns atributos e métodos na definição UML da classe Escopo
</commit_message>
<xml_diff>
--- a/UML.xlsx
+++ b/UML.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git dev\prog1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
   <si>
     <t>Escopo</t>
   </si>
@@ -85,22 +90,29 @@
   </si>
   <si>
     <t>setValor(String t)</t>
+  </si>
+  <si>
+    <t>String[] ??</t>
+  </si>
+  <si>
+    <t>comandos</t>
+  </si>
+  <si>
+    <t>ArrayList</t>
+  </si>
+  <si>
+    <t>variaveis</t>
+  </si>
+  <si>
+    <t>processa()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -339,15 +351,6 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -384,19 +387,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,6 +418,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -647,7 +662,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -682,7 +697,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -893,13 +908,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="6" width="14.140625" customWidth="1"/>
+    <col min="4" max="6" width="14.140625" style="20" customWidth="1"/>
     <col min="10" max="11" width="14.140625" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="14.140625" customWidth="1"/>
@@ -908,224 +921,236 @@
   <sheetData>
     <row r="2" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="M3" s="16" t="s">
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="M3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="17"/>
-      <c r="O3" s="18"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="4:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="M4" s="6" t="s">
+      <c r="D4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="E4" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="M5" s="11" t="s">
+      <c r="D5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="E5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="4:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="M7" s="9" t="s">
+      <c r="D7" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="O7" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="M8" s="9" t="s">
+      <c r="M8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N9" s="12" t="s">
+      <c r="N9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O9" s="13" t="s">
+      <c r="O9" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="4:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="4:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="18"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="16"/>
     </row>
     <row r="13" spans="4:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L13" s="14" t="s">
+      <c r="L13" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="4:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="L15" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="10:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="10:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J18" s="16" t="s">
+      <c r="J18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="17"/>
-      <c r="L18" s="18"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
     </row>
     <row r="19" spans="10:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="K19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L19" s="14" t="s">
+      <c r="L19" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="10:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="J20" s="6" t="s">
+      <c r="J20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L20" s="8" t="s">
+      <c r="L20" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J21" s="9" t="s">
+      <c r="J21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L21" s="10" t="s">
+      <c r="L21" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="19"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="13"/>
     </row>
     <row r="23" spans="10:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="10:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J24" s="16" t="s">
+      <c r="J24" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="18"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="16"/>
     </row>
     <row r="25" spans="10:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J25" s="6" t="s">
+      <c r="J25" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L25" s="14" t="s">
+      <c r="L25" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="10:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="J26" s="6" t="s">
+      <c r="J26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K26" s="7" t="s">
+      <c r="K26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L26" s="8" t="s">
+      <c r="L26" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="27" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J27" s="9" t="s">
+      <c r="J27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L27" s="10" t="s">
+      <c r="L27" s="7" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- adicionados mais alguns protótipos de métodos na definição UML da classe "Escopo"
</commit_message>
<xml_diff>
--- a/UML.xlsx
+++ b/UML.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>Escopo</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>processa()</t>
+  </si>
+  <si>
+    <t>getVariaveis()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">void </t>
+  </si>
+  <si>
+    <t>setVariaveis(Variavel[] vars)</t>
+  </si>
+  <si>
+    <t>addVariavel(Variavel var)</t>
   </si>
 </sst>
 </file>
@@ -137,6 +149,187 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -144,20 +337,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -168,203 +348,38 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,43 +387,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -908,11 +916,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:F18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="6" width="14.140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="17" customWidth="1"/>
     <col min="10" max="11" width="14.140625" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="14.140625" customWidth="1"/>
@@ -921,11 +933,11 @@
   <sheetData>
     <row r="2" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
       <c r="M3" s="14" t="s">
         <v>1</v>
       </c>
@@ -933,13 +945,13 @@
       <c r="O3" s="16"/>
     </row>
     <row r="4" spans="4:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="21" t="s">
         <v>24</v>
       </c>
       <c r="M4" s="3" t="s">
@@ -953,13 +965,13 @@
       </c>
     </row>
     <row r="5" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="21" t="s">
         <v>26</v>
       </c>
       <c r="M5" s="8" t="s">
@@ -973,6 +985,9 @@
       </c>
     </row>
     <row r="6" spans="4:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
       <c r="M6" s="3" t="s">
         <v>7</v>
       </c>
@@ -984,13 +999,13 @@
       </c>
     </row>
     <row r="7" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="21" t="s">
         <v>27</v>
       </c>
       <c r="M7" s="6" t="s">
@@ -1004,6 +1019,15 @@
       </c>
     </row>
     <row r="8" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D8" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="M8" s="6" t="s">
         <v>7</v>
       </c>
@@ -1015,6 +1039,15 @@
       </c>
     </row>
     <row r="9" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>30</v>
+      </c>
       <c r="M9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1025,7 +1058,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="4:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="4:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="11" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="4:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J12" s="14" t="s">

</xml_diff>